<commit_message>
db update, manage updates
</commit_message>
<xml_diff>
--- a/app/public/static/aktemp-files-template.xlsx
+++ b/app/public/static/aktemp-files-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/git/ecosheds/aktemp/app/public/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF85F73-2A59-8E4B-9164-12CA46ED1816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FFDD33-CA23-3642-B099-1607150C7751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="500" windowWidth="48220" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="125">
   <si>
     <t>Updated:</t>
   </si>
@@ -45,30 +45,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Archangel</t>
-  </si>
-  <si>
-    <t>Archangel-20431778.csv</t>
-  </si>
-  <si>
-    <t>Archangel-20689953.csv</t>
-  </si>
-  <si>
-    <t>Coal Creek</t>
-  </si>
-  <si>
-    <t>Coal Creek-20689995.csv</t>
-  </si>
-  <si>
-    <t>Coho Creek-20431771.csv</t>
-  </si>
-  <si>
-    <t>Coho Creek-20689952.csv</t>
-  </si>
-  <si>
-    <t>Fish Hook Creek-20861232.csv</t>
-  </si>
-  <si>
     <t>datetime</t>
   </si>
   <si>
@@ -120,22 +96,10 @@
     <t>MID-DEPTH</t>
   </si>
   <si>
-    <t>-999,NA</t>
-  </si>
-  <si>
     <t>flag</t>
   </si>
   <si>
     <t>STATION</t>
-  </si>
-  <si>
-    <t>station</t>
-  </si>
-  <si>
-    <t>BOTTOM</t>
-  </si>
-  <si>
-    <t>SURFACE</t>
   </si>
   <si>
     <t>temp_f</t>
@@ -454,7 +418,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -1118,7 +1082,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1154,7 +1118,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1175,96 +1139,95 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1743,8 +1706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1760,14 +1723,14 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="50">
+      <c r="B3" s="37">
         <v>44812</v>
       </c>
     </row>
@@ -1780,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1788,15 +1751,15 @@
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
+      <c r="A7" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -1807,37 +1770,37 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="4" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1847,395 +1810,395 @@
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="41" t="s">
+      <c r="B16" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="45" t="s">
-        <v>59</v>
+      <c r="B17" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="32" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>63</v>
+      <c r="B18" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="40" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="47" t="s">
-        <v>106</v>
+      <c r="B19" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="40" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="43"/>
-      <c r="E20" s="47" t="s">
-        <v>105</v>
+      <c r="B20" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="34" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="40" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="46"/>
-      <c r="E21" s="45" t="s">
-        <v>67</v>
+      <c r="B21" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="33"/>
+      <c r="E21" s="32" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="40" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="31"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="80" x14ac:dyDescent="0.25">
+      <c r="B24" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="33"/>
+      <c r="E24" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="B25" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="33"/>
+      <c r="E25" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="B26" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="30"/>
+      <c r="E26" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="K26" s="13"/>
+    </row>
+    <row r="27" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="B27" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="B28" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="31"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="80" x14ac:dyDescent="0.25">
+      <c r="B29" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="31"/>
+      <c r="D29" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="B30" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="33"/>
+      <c r="E30" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B31" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="B32" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="31"/>
+      <c r="D32" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="B33" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="31"/>
+      <c r="D33" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="80" x14ac:dyDescent="0.25">
+      <c r="B34" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="45" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="46" t="s">
+      <c r="C34" s="31"/>
+      <c r="D34" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="32" t="s">
         <v>91</v>
-      </c>
-      <c r="E23" s="45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="80" x14ac:dyDescent="0.25">
-      <c r="B24" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="45" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="80" x14ac:dyDescent="0.25">
-      <c r="B25" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="B26" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" s="46"/>
-      <c r="E26" s="45" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B27" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="43"/>
-      <c r="E27" s="45" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="B28" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="46"/>
-      <c r="E28" s="45" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="B29" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="K29" s="13"/>
-    </row>
-    <row r="30" spans="1:11" ht="40" x14ac:dyDescent="0.25">
-      <c r="B30" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="45" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="40" x14ac:dyDescent="0.25">
-      <c r="B31" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="40" x14ac:dyDescent="0.25">
-      <c r="B32" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" s="45" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="40" x14ac:dyDescent="0.25">
-      <c r="B33" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" s="45" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="80" x14ac:dyDescent="0.25">
-      <c r="B34" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" s="45" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="45"/>
+    </row>
+    <row r="37" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="24"/>
+      <c r="C37" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="47"/>
+    </row>
+    <row r="38" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="25"/>
+      <c r="C38" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="49"/>
+    </row>
+    <row r="39" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" s="45"/>
+    </row>
+    <row r="40" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="25"/>
+      <c r="C40" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="49"/>
+    </row>
+    <row r="41" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="45"/>
+    </row>
+    <row r="42" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="26"/>
+      <c r="C42" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="47"/>
+    </row>
+    <row r="43" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="27"/>
+      <c r="C43" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="49"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="30"/>
-    </row>
-    <row r="37" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="36"/>
-      <c r="C37" s="18" t="s">
+      <c r="E44" s="45"/>
+    </row>
+    <row r="45" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="26"/>
+      <c r="C45" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="31"/>
-    </row>
-    <row r="38" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="37"/>
-      <c r="C38" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="E38" s="32"/>
-    </row>
-    <row r="39" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="35" t="s">
+      <c r="D45" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="30"/>
-    </row>
-    <row r="40" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="37"/>
-      <c r="C40" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" s="32"/>
-    </row>
-    <row r="41" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="30"/>
-    </row>
-    <row r="42" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="38"/>
-      <c r="C42" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="31"/>
-    </row>
-    <row r="43" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="39"/>
-      <c r="C43" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="E43" s="32"/>
-      <c r="F43" s="12"/>
-    </row>
-    <row r="44" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E44" s="30"/>
-    </row>
-    <row r="45" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="38"/>
-      <c r="C45" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D45" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="31"/>
+      <c r="E45" s="47"/>
     </row>
     <row r="46" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="39"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="32"/>
+        <v>22</v>
+      </c>
+      <c r="D46" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="49"/>
     </row>
     <row r="47" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="38" t="s">
-        <v>95</v>
+      <c r="B47" s="26" t="s">
+        <v>83</v>
       </c>
       <c r="C47" s="15">
         <v>1</v>
       </c>
-      <c r="D47" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="E47" s="33"/>
+      <c r="D47" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" s="51"/>
     </row>
     <row r="48" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="20"/>
       <c r="C48" s="15">
         <v>2</v>
       </c>
-      <c r="D48" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="E48" s="34"/>
+      <c r="D48" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" s="40"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="21"/>
-      <c r="C49" s="24">
+      <c r="C49" s="22">
         <v>3</v>
       </c>
-      <c r="D49" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E49" s="23"/>
+      <c r="D49" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2267,273 +2230,121 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="8" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" style="8" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="L1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="M1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="Q1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="R1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="8">
-        <v>-9</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="8">
-        <v>-9999</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" s="7" t="b">
-        <v>1</v>
-      </c>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="8">
-        <v>-8</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="8">
-        <v>5</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" s="7" t="b">
-        <v>0</v>
-      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="K3" s="11"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="8">
-        <v>-7</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="7">
-        <v>3</v>
-      </c>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="G5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="G6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="G7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -2735,11 +2546,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49586CA0-D21C-204E-A207-ACD740665BED}">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2753,13 +2564,13 @@
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -2767,109 +2578,109 @@
   <sheetData>
     <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="M1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="N1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="R1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="S1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="U1" s="48" t="s">
-        <v>109</v>
+      <c r="U1" s="35" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="176" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>114</v>
+      <c r="A2" s="36" t="s">
+        <v>102</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I2" s="8">
         <v>-9</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="L2" s="8">
+        <v>-9999</v>
+      </c>
+      <c r="M2" s="8"/>
       <c r="N2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="8">
-        <v>-9999</v>
-      </c>
-      <c r="P2" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="7"/>
       <c r="Q2" s="7">
         <v>1</v>
       </c>
@@ -2881,48 +2692,48 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="198" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
-        <v>117</v>
+      <c r="A3" s="36" t="s">
+        <v>105</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="P3" s="8"/>
+      <c r="O3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="7" t="b">
         <v>0</v>
@@ -2932,51 +2743,51 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="198" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
-        <v>115</v>
+      <c r="A4" s="36" t="s">
+        <v>103</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I4" s="8">
         <v>-8</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="8">
+        <v>9</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="8">
+        <v>-9999</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="8">
         <v>1</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="8">
-        <v>-9999</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>33</v>
+      <c r="P4" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="Q4" s="7">
         <v>1</v>
@@ -2989,91 +2800,91 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="149" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
-        <v>128</v>
+      <c r="A5" s="36" t="s">
+        <v>116</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="I5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="K5" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>38</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L5" s="8"/>
+      <c r="M5" s="11"/>
       <c r="N5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:21" ht="155" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
-        <v>118</v>
+      <c r="A6" s="36" t="s">
+        <v>106</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I6" s="8">
         <v>-8</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" s="11"/>
-      <c r="P6" s="8"/>
+      <c r="J6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="11"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7" t="b">

</xml_diff>

<commit_message>
add rds proxy, manage views
</commit_message>
<xml_diff>
--- a/app/public/static/aktemp-files-template.xlsx
+++ b/app/public/static/aktemp-files-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/git/ecosheds/aktemp/app/public/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B38C04-9F0D-BE46-80A5-830567A31B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239893A6-466C-BF4C-B0FC-8DD394C606C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="500" windowWidth="48220" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1194,6 +1194,45 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1209,50 +1248,11 @@
     <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1783,12 +1783,12 @@
       <c r="A7" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -1958,7 +1958,7 @@
       <c r="C24" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="50" t="s">
+      <c r="D24" s="39" t="s">
         <v>111</v>
       </c>
       <c r="E24" s="29" t="s">
@@ -2064,28 +2064,28 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="40" x14ac:dyDescent="0.25">
       <c r="B33" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="27"/>
+      <c r="E33" s="29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="B34" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="30" t="s">
+      <c r="C34" s="28"/>
+      <c r="D34" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="E34" s="29" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="40" x14ac:dyDescent="0.25">
-      <c r="B34" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="29" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="40" x14ac:dyDescent="0.25">
@@ -2134,33 +2134,33 @@
       <c r="C39" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="39" t="s">
+      <c r="D39" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="40"/>
+      <c r="E39" s="44"/>
     </row>
     <row r="40" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="22"/>
       <c r="C40" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="41" t="s">
+      <c r="D40" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="42"/>
+      <c r="E40" s="46"/>
     </row>
     <row r="41" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="23"/>
       <c r="C41" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="43" t="s">
+      <c r="D41" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="E41" s="44"/>
+      <c r="E41" s="53"/>
     </row>
     <row r="42" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="40" t="s">
         <v>46</v>
       </c>
       <c r="C42" s="15" t="s">
@@ -2172,34 +2172,34 @@
       <c r="E42" s="55"/>
     </row>
     <row r="43" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="52"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="41" t="s">
+      <c r="D43" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="E43" s="42"/>
+      <c r="E43" s="46"/>
     </row>
     <row r="44" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="52"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="41" t="s">
+      <c r="D44" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="E44" s="42"/>
+      <c r="E44" s="46"/>
     </row>
     <row r="45" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="53"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="43" t="s">
+      <c r="D45" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="44"/>
+      <c r="E45" s="53"/>
       <c r="F45" s="12"/>
     </row>
     <row r="46" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -2209,32 +2209,32 @@
       <c r="C46" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D46" s="39" t="s">
+      <c r="D46" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="E46" s="40"/>
+      <c r="E46" s="44"/>
       <c r="F46" s="12"/>
     </row>
     <row r="47" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="52"/>
+      <c r="B47" s="41"/>
       <c r="C47" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="41" t="s">
+      <c r="D47" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="E47" s="42"/>
+      <c r="E47" s="46"/>
       <c r="F47" s="12"/>
     </row>
     <row r="48" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="53"/>
+      <c r="B48" s="42"/>
       <c r="C48" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D48" s="43" t="s">
+      <c r="D48" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="E48" s="44"/>
+      <c r="E48" s="53"/>
       <c r="F48" s="12"/>
     </row>
     <row r="49" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -2244,30 +2244,30 @@
       <c r="C49" s="14">
         <v>1</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D49" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="E49" s="35"/>
+      <c r="E49" s="48"/>
     </row>
     <row r="50" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="18"/>
       <c r="C50" s="14">
         <v>2</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D50" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="E50" s="35"/>
+      <c r="E50" s="48"/>
     </row>
     <row r="51" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="19"/>
       <c r="C51" s="20">
         <v>3</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="D51" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="37"/>
+      <c r="E51" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2301,12 +2301,12 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" style="8" bestFit="1" customWidth="1"/>
@@ -2322,8 +2322,8 @@
     <col min="14" max="14" width="15" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20" style="7" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
@@ -2380,10 +2380,10 @@
         <v>99</v>
       </c>
       <c r="Q1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="S1" s="10" t="s">
         <v>35</v>
@@ -2633,14 +2633,14 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="67.6640625" customWidth="1"/>
-    <col min="2" max="2" width="40.5" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="37" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
@@ -2655,15 +2655,15 @@
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -2715,10 +2715,10 @@
         <v>99</v>
       </c>
       <c r="R1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="T1" s="10" t="s">
         <v>35</v>
@@ -2731,10 +2731,10 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="176" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="38" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="8">
@@ -2746,7 +2746,7 @@
       <c r="E2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="48"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
@@ -2771,9 +2771,9 @@
       <c r="P2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="8"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="37"/>
       <c r="T2" s="8">
         <v>1</v>
       </c>
@@ -2785,10 +2785,10 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="242" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="38" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="8">
@@ -2800,7 +2800,7 @@
       <c r="E3" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="48"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="8" t="s">
         <v>7</v>
       </c>
@@ -2823,10 +2823,10 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="T3" s="8"/>
       <c r="U3" s="8" t="b">
@@ -2837,10 +2837,10 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="198" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="38" t="s">
         <v>78</v>
       </c>
       <c r="C4" s="8">
@@ -2880,10 +2880,10 @@
       <c r="Q4" s="8">
         <v>1</v>
       </c>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="S4" s="8"/>
       <c r="T4" s="8">
         <v>1</v>
       </c>
@@ -2895,10 +2895,10 @@
       </c>
     </row>
     <row r="5" spans="1:22" ht="149" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="38" t="s">
         <v>80</v>
       </c>
       <c r="C5" s="8">
@@ -2910,7 +2910,7 @@
       <c r="E5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="8" t="s">
         <v>7</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="I5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="48"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="8" t="s">
         <v>18</v>
       </c>
@@ -2931,22 +2931,22 @@
       <c r="N5" s="8"/>
       <c r="O5" s="11"/>
       <c r="P5" s="8"/>
-      <c r="Q5" s="48"/>
+      <c r="Q5" s="37"/>
       <c r="R5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="S5" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
     </row>
     <row r="6" spans="1:22" ht="155" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="38" t="s">
         <v>79</v>
       </c>
       <c r="C6" s="8">
@@ -2958,7 +2958,7 @@
       <c r="E6" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="48"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="8" t="s">
         <v>14</v>
       </c>

</xml_diff>